<commit_message>
with hackaday links to step files
</commit_message>
<xml_diff>
--- a/hardware/uven2-mk3.xlsx
+++ b/hardware/uven2-mk3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letrend\Documents\UVen\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CACE290-B814-4A52-AF25-89FA7E8B6435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7E1D8E-F429-490B-9418-D5C26AD6A48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="145">
   <si>
     <t xml:space="preserve">part </t>
   </si>
@@ -89,9 +89,6 @@
     <t>led_base</t>
   </si>
   <si>
-    <t>chamber_front</t>
-  </si>
-  <si>
     <t>chamber_back</t>
   </si>
   <si>
@@ -107,21 +104,12 @@
     <t>chamber_right_1</t>
   </si>
   <si>
-    <t>control_panel_top</t>
-  </si>
-  <si>
-    <t>interlock_case_a</t>
-  </si>
-  <si>
     <t>endstop</t>
   </si>
   <si>
     <t>exhaust_shield</t>
   </si>
   <si>
-    <t>control_panel_bottom</t>
-  </si>
-  <si>
     <t>handle</t>
   </si>
   <si>
@@ -146,9 +134,6 @@
     <t>chamber_plug</t>
   </si>
   <si>
-    <t>shipping costs</t>
-  </si>
-  <si>
     <t>E200-R22-C10R</t>
   </si>
   <si>
@@ -336,18 +321,167 @@
   </si>
   <si>
     <t>https://github.com/letrend/UVen/blob/uven2_mk3/hardware/uven2-mk3-cc-driver-25x.eprj</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/exhaust_shield.step</t>
+  </si>
+  <si>
+    <t>display_mount_bottom</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/display_mount_bottom.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_left_1.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/left_lower.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/base.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_right_1.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_front_left.step</t>
+  </si>
+  <si>
+    <t>chamber_front_left</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/endstop.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/spacer_top_right.step</t>
+  </si>
+  <si>
+    <t>interlock_case_a1</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/interlock_case_a.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_back.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/right_lower.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_right_0.step</t>
+  </si>
+  <si>
+    <t>chamber_hinge_lock_front_right</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_hinge_lock_front_right.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/power_supply_holder_0.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/lid.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/top_cover_right.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/hinge_left_lock.step</t>
+  </si>
+  <si>
+    <t>chamber_hinge_front</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_hinge_front.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/hinge_right.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/driver_right.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/top_cover_left.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_left_0.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/handle.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/driver_left.step</t>
+  </si>
+  <si>
+    <t>chamber_front_right</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_front_right.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/spacer_right_lower.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/fan_protection.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/led_base.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/front_lower.step</t>
+  </si>
+  <si>
+    <t>chamber_hinge_lock_front_left</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_hinge_lock_front_left.step</t>
+  </si>
+  <si>
+    <t>spacer_top_left</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/spacer_top_left.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/back_lower.step</t>
+  </si>
+  <si>
+    <t>display_mount_top</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/display_mount_top.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/hinge_right_lock.step</t>
+  </si>
+  <si>
+    <t>spacer_left_lower</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/spacer_left_lower.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/chamber_plug.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/interlock_case_b.step</t>
+  </si>
+  <si>
+    <t>https://cdn.hackaday.io/files/2031988693623232/hinge_left.step</t>
+  </si>
+  <si>
+    <t>shipping costs+customs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€];[Red]\-#,##0.00\ [$€]"/>
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -369,6 +503,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,15 +533,16 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -738,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,870 +903,1056 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>25.56</v>
+      <c r="C2" s="6">
+        <v>19.43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>25.56</v>
+      <c r="C3" s="6">
+        <v>4.13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>34.92</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>38.520000000000003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>8.1300000000000008</v>
+      <c r="C5" s="6">
+        <v>29.15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
-        <v>7.37</v>
+      <c r="C6" s="6">
+        <v>18.43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>10.92</v>
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>28.84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>11.5</v>
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="E8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
-        <v>18.43</v>
+      <c r="C9" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
-        <v>11.49</v>
+      <c r="C10" s="6">
+        <v>8.66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
-        <v>22.98</v>
+      <c r="C11" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="E11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
-        <v>38.64</v>
+      <c r="C12" s="6">
+        <v>25.59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1">
-        <v>17.71</v>
+      <c r="C13" s="6">
+        <v>38.520000000000003</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
-        <v>17.71</v>
+      <c r="C14" s="6">
+        <v>20.53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="1">
-        <v>28.43</v>
+      <c r="C15" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>13.63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <f>4*13.14</f>
+        <v>52.56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>17.71</v>
+      </c>
+      <c r="E17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
+        <v>7.71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="E21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6">
+        <v>36.18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6">
+        <v>6.89</v>
+      </c>
+      <c r="E23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>27.28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1">
-        <v>10.96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>10.96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1">
-        <v>30.79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1">
-        <v>30.79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>11.21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6">
+        <v>10.41</v>
+      </c>
+      <c r="E24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
       <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1">
-        <v>16.72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="6">
+        <f>2*0.86</f>
+        <v>1.72</v>
+      </c>
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="1">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
+      <c r="C26" s="6">
+        <v>36.18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="6">
+        <v>11.86</v>
+      </c>
+      <c r="E27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="E28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="6">
+        <v>5.96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="6">
+        <v>27.07</v>
+      </c>
+      <c r="E30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="6">
+        <v>44.98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="1">
-        <v>0.85</v>
+      <c r="C32" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="E32" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1">
-        <v>4.7300000000000004</v>
+        <v>2</v>
+      </c>
+      <c r="C33" s="6">
+        <v>8.66</v>
+      </c>
+      <c r="E33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" s="1">
-        <v>2.76</v>
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
+        <v>48.86</v>
+      </c>
+      <c r="E34" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="1">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="E35" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" s="2">
-        <v>33.93</v>
+      <c r="C36" s="6">
+        <v>0.86</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2">
-        <f>5.95*B37</f>
-        <v>11.9</v>
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>8.8800000000000008</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2">
-        <v>38.619999999999997</v>
+        <v>2</v>
+      </c>
+      <c r="C38" s="6">
+        <f>2*1.52</f>
+        <v>3.04</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2">
-        <f>4.42*B39</f>
-        <v>17.68</v>
+        <v>1</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.86</v>
       </c>
       <c r="E39" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="2">
-        <v>27.25</v>
+      <c r="C40" s="6">
+        <v>0.86</v>
       </c>
       <c r="E40" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41" s="2">
-        <f>81.27*B41</f>
-        <v>325.08</v>
-      </c>
-      <c r="E41" t="s">
-        <v>48</v>
+        <v>144</v>
+      </c>
+      <c r="C41" s="6">
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42" s="2">
-        <v>387.69</v>
+      <c r="C42" s="1">
+        <v>33.93</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2">
-        <v>104.92</v>
+        <v>2</v>
+      </c>
+      <c r="C43" s="1">
+        <f>5.95*B43</f>
+        <v>11.9</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44" s="2">
-        <v>334.91</v>
+        <v>1</v>
+      </c>
+      <c r="C44" s="1">
+        <v>38.619999999999997</v>
       </c>
       <c r="E44" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2">
-        <v>78.260000000000005</v>
+        <v>4</v>
+      </c>
+      <c r="C45" s="1">
+        <f>4.42*B45</f>
+        <v>17.68</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
-      <c r="C46" s="2">
-        <v>76.11</v>
+      <c r="C46" s="1">
+        <v>27.25</v>
       </c>
       <c r="E46" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C47" s="1">
-        <v>109.71</v>
+        <f>81.27*B47</f>
+        <v>325.08</v>
       </c>
       <c r="E47" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>56</v>
+      <c r="A48" t="s">
+        <v>44</v>
       </c>
       <c r="B48">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C48" s="1">
-        <f>8.74*B48</f>
-        <v>874</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>57</v>
+        <v>387.69</v>
+      </c>
+      <c r="E48" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" s="2">
-        <v>36.47</v>
+      <c r="C49" s="1">
+        <v>104.92</v>
       </c>
       <c r="E49" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B50">
-        <v>20</v>
-      </c>
-      <c r="C50" s="2">
-        <v>6.07</v>
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>334.91</v>
       </c>
       <c r="E50" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>22</v>
-      </c>
-      <c r="C51" s="2">
-        <v>6.66</v>
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>78.260000000000005</v>
       </c>
       <c r="E51" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>350</v>
-      </c>
-      <c r="C52" s="2">
-        <v>9.08</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>83</v>
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>76.11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B53">
-        <v>6</v>
-      </c>
-      <c r="C53" s="2">
-        <v>8.6300000000000008</v>
+        <v>1</v>
+      </c>
+      <c r="C53" s="6">
+        <v>109.71</v>
       </c>
       <c r="E53" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>66</v>
+      <c r="A54" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B54">
-        <v>4</v>
-      </c>
-      <c r="C54" s="2">
-        <v>10.99</v>
-      </c>
-      <c r="E54" t="s">
-        <v>67</v>
+        <v>100</v>
+      </c>
+      <c r="C54" s="6">
+        <f>8.74*B54</f>
+        <v>874</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>8</v>
-      </c>
-      <c r="C55" s="2">
-        <v>7.99</v>
+        <v>1</v>
+      </c>
+      <c r="C55" s="1">
+        <v>36.47</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B56">
-        <v>2</v>
-      </c>
-      <c r="C56" s="2">
-        <f>1.05*B56</f>
-        <v>2.1</v>
+        <v>20</v>
+      </c>
+      <c r="C56" s="1">
+        <v>6.07</v>
       </c>
       <c r="E56" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B57">
-        <v>12</v>
-      </c>
-      <c r="C57" s="2">
-        <v>11.31</v>
+        <v>22</v>
+      </c>
+      <c r="C57" s="1">
+        <v>6.66</v>
       </c>
       <c r="E57" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B58">
-        <v>15</v>
-      </c>
-      <c r="C58" s="2">
-        <v>8.59</v>
-      </c>
-      <c r="E58" t="s">
-        <v>74</v>
+        <v>350</v>
+      </c>
+      <c r="C58" s="1">
+        <v>9.08</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B59">
-        <v>17</v>
-      </c>
-      <c r="C59" s="2">
-        <v>3.78</v>
+        <v>6</v>
+      </c>
+      <c r="C59" s="1">
+        <v>8.6300000000000008</v>
       </c>
       <c r="E59" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B60">
-        <v>10</v>
-      </c>
-      <c r="C60" s="2">
-        <v>7.84</v>
+        <v>4</v>
+      </c>
+      <c r="C60" s="1">
+        <v>10.99</v>
       </c>
       <c r="E60" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="C61" s="2">
-        <v>9.8800000000000008</v>
+        <v>8</v>
+      </c>
+      <c r="C61" s="1">
+        <v>7.99</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B62">
-        <v>8</v>
-      </c>
-      <c r="C62" s="2">
-        <v>5.33</v>
+        <v>2</v>
+      </c>
+      <c r="C62" s="1">
+        <f>1.05*B62</f>
+        <v>2.1</v>
       </c>
       <c r="E62" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B63">
-        <v>6</v>
-      </c>
-      <c r="C63" s="2">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="C63" s="1">
+        <v>11.31</v>
       </c>
       <c r="E63" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" s="2">
-        <v>32.64</v>
+        <v>15</v>
+      </c>
+      <c r="C64" s="1">
+        <v>8.59</v>
       </c>
       <c r="E64" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B65">
-        <v>2</v>
-      </c>
-      <c r="C65" s="2">
-        <v>17.32</v>
+        <v>17</v>
+      </c>
+      <c r="C65" s="1">
+        <v>3.78</v>
       </c>
       <c r="E65" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" s="2">
-        <v>1.19</v>
+        <v>10</v>
+      </c>
+      <c r="C66" s="1">
+        <v>7.84</v>
       </c>
       <c r="E66" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B67">
-        <v>100</v>
-      </c>
-      <c r="C67" s="2">
-        <v>0.1</v>
+        <v>4</v>
+      </c>
+      <c r="C67" s="1">
+        <v>9.8800000000000008</v>
       </c>
       <c r="E67" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B68">
-        <v>100</v>
-      </c>
-      <c r="C68" s="2">
-        <v>0.05</v>
+        <v>8</v>
+      </c>
+      <c r="C68" s="1">
+        <v>5.33</v>
       </c>
       <c r="E68" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" s="2">
+        <v>6</v>
+      </c>
+      <c r="C69" s="1">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1">
+        <v>32.64</v>
+      </c>
+      <c r="E70" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" s="1">
+        <v>17.32</v>
+      </c>
+      <c r="E71" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1.19</v>
+      </c>
+      <c r="E72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73">
+        <v>100</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B74">
+        <v>100</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C74" s="4">
-        <f>SUM(C2:C73)</f>
-        <v>3230.36</v>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C80" s="3">
+        <f>SUM(C2:C79)</f>
+        <v>3521.6000000000004</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E52" r:id="rId1" xr:uid="{FFA81BDA-DD74-4D64-A280-914C50CBA945}"/>
-    <hyperlink ref="E48" r:id="rId2" xr:uid="{D802E364-6A6E-4536-B3D3-A5BC67583CD7}"/>
+    <hyperlink ref="E58" r:id="rId1" xr:uid="{FFA81BDA-DD74-4D64-A280-914C50CBA945}"/>
+    <hyperlink ref="E54" r:id="rId2" xr:uid="{D802E364-6A6E-4536-B3D3-A5BC67583CD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>